<commit_message>
Removed auto increment from id columns as the ID is being read from the excel sheel and added manually
</commit_message>
<xml_diff>
--- a/HibernateExam110424/src/main/resources/Exam_info.xlsx
+++ b/HibernateExam110424/src/main/resources/Exam_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZorbaExamSubmission\HibernateExam110424\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF5D97E-A874-4EFD-A3E2-BA37528A5223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D7310C-7E0A-478F-A1A6-05E205CBAFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{AA7A81E4-0C64-4AC8-A414-7B6FB661CF94}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{AA7A81E4-0C64-4AC8-A414-7B6FB661CF94}"/>
   </bookViews>
   <sheets>
     <sheet name="employee" sheetId="1" r:id="rId1"/>
@@ -834,10 +834,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3178ACF-6003-4F4B-A644-8C62CC32BF99}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4">
         <v>1004</v>
@@ -879,93 +879,88 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5">
-        <v>1001</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6">
-        <v>1003</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
-        <v>1001</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B13">
-        <v>1004</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B14">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>104</v>
-      </c>
-      <c r="B15">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+    <sortCondition ref="A1:A14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>